<commit_message>
Highlight user API commit
</commit_message>
<xml_diff>
--- a/db/APIs.xlsx
+++ b/db/APIs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -129,12 +129,6 @@
   </si>
   <si>
     <t>PUT</t>
-  </si>
-  <si>
-    <t>Show featured images</t>
-  </si>
-  <si>
-    <t>http://celebritybe.local/api/v1/userimages</t>
   </si>
   <si>
     <t>Config items</t>
@@ -266,12 +260,40 @@
   <si>
     <t>{from:1; to:2; chat_text: text, chat_on: date_time}</t>
   </si>
+  <si>
+    <t xml:space="preserve">Highlighted Users </t>
+  </si>
+  <si>
+    <t>http://celebritybe.local/api/v1/highlightusers</t>
+  </si>
+  <si>
+    <t>http://celebritybe.local/api/v1/usermedias</t>
+  </si>
+  <si>
+    <t>Show featured media</t>
+  </si>
+  <si>
+    <t>Add featured media</t>
+  </si>
+  <si>
+    <t>{
+"user_id" : " user id ",
+"user_video" :['video urls in array format'],
+"user_image" : ['base64 image data in array format']
+}</t>
+  </si>
+  <si>
+    <t>ACCESS-TOKEN = access token string</t>
+  </si>
+  <si>
+    <t>Plan read</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -295,8 +317,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +335,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8EB4E3"/>
         <bgColor rgb="FF9999FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -323,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,14 +377,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -710,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -731,68 +808,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1">
+    <row r="2" spans="1:9" s="9" customFormat="1">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
+    <row r="3" spans="1:9" s="9" customFormat="1">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="7"/>
@@ -800,127 +877,135 @@
       <c r="G3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
+    <row r="4" spans="1:9" s="9" customFormat="1">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="8"/>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="9" customFormat="1">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1">
+    <row r="7" spans="1:9" s="9" customFormat="1">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="20">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1">
+      <c r="G8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" s="9" customFormat="1">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="7"/>
@@ -928,185 +1013,292 @@
         <v>20</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="H9" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1">
+    <row r="10" spans="1:9" s="9" customFormat="1">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1">
+    <row r="11" spans="1:9" s="9" customFormat="1">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1">
+    <row r="12" spans="1:9" s="9" customFormat="1">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="1">
+      <c r="A13" s="20">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="20">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="20">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="20">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="G16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="20">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="20">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="20">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="C19" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="G19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="D20" s="15"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="20">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="20">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="C22" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="C24" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1114,22 +1306,26 @@
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5"/>
-    <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="C9" r:id="rId7"/>
-    <hyperlink ref="C13" r:id="rId8"/>
-    <hyperlink ref="C12" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C14" r:id="rId11"/>
-    <hyperlink ref="C15" r:id="rId12"/>
-    <hyperlink ref="C16" r:id="rId13"/>
-    <hyperlink ref="C17" r:id="rId14"/>
-    <hyperlink ref="C19" r:id="rId15"/>
-    <hyperlink ref="C18" r:id="rId16"/>
+    <hyperlink ref="C9" r:id="rId5"/>
+    <hyperlink ref="C10" r:id="rId6"/>
+    <hyperlink ref="C11" r:id="rId7"/>
+    <hyperlink ref="C16" r:id="rId8"/>
+    <hyperlink ref="C15" r:id="rId9"/>
+    <hyperlink ref="C14" r:id="rId10"/>
+    <hyperlink ref="C17" r:id="rId11"/>
+    <hyperlink ref="C18" r:id="rId12"/>
+    <hyperlink ref="C19" r:id="rId13"/>
+    <hyperlink ref="C20" r:id="rId14"/>
+    <hyperlink ref="C21" r:id="rId15"/>
+    <hyperlink ref="C22" r:id="rId16" display="http://celebritybe.local/api/v1/interviews"/>
     <hyperlink ref="C6" r:id="rId17"/>
+    <hyperlink ref="C13" r:id="rId18"/>
+    <hyperlink ref="C7" r:id="rId19" display="http://celebritybe.local/api/v1/userimages"/>
+    <hyperlink ref="C8" r:id="rId20" display="http://celebritybe.local/api/v1/userimages"/>
+    <hyperlink ref="C12" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Interest api and usermedia api file commit:
</commit_message>
<xml_diff>
--- a/db/APIs.xlsx
+++ b/db/APIs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t>#</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>{from:1; to:2;}</t>
-  </si>
-  <si>
-    <t>http://celebritybe.local/api/v1/send_interest</t>
   </si>
   <si>
     <t>http://celebritybe.local/api/v1/interests</t>
@@ -363,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,6 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -900,7 +898,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7"/>
@@ -921,7 +919,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -931,10 +929,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>54</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>19</v>
@@ -944,7 +942,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -954,20 +952,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -977,10 +975,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>19</v>
@@ -990,7 +988,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1036,7 +1034,7 @@
         <v>20</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1059,7 +1057,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1069,7 +1067,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>27</v>
@@ -1082,7 +1080,7 @@
         <v>20</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -1103,7 +1101,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1116,7 +1114,7 @@
         <v>33</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="5"/>
@@ -1124,33 +1122,33 @@
         <v>36</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="20">
+    <row r="15" spans="1:9" s="9" customFormat="1">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="G15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1">
       <c r="A16" s="11">
@@ -1159,7 +1157,7 @@
       <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -1170,7 +1168,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1183,13 +1181,13 @@
         <v>31</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1199,10 +1197,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="5"/>
@@ -1210,7 +1208,7 @@
         <v>36</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1220,18 +1218,18 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1241,18 +1239,18 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1265,7 +1263,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="5"/>
@@ -1273,7 +1271,7 @@
         <v>36</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1283,18 +1281,18 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>50</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>

</xml_diff>

<commit_message>
User chat api commit:
</commit_message>
<xml_diff>
--- a/db/APIs.xlsx
+++ b/db/APIs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
   <si>
     <t>#</t>
   </si>
@@ -240,12 +240,6 @@
     <t>http://celebritybe.local/api/v1/chat-users</t>
   </si>
   <si>
-    <t>http://celebritybe.local/api/v1/chat-msg</t>
-  </si>
-  <si>
-    <t>http://celebritybe.local/api/v1/chat-submit</t>
-  </si>
-  <si>
     <t>Send Interview letters</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
   </si>
   <si>
     <t>http://celebritybe.local/api/v1/interviews</t>
-  </si>
-  <si>
-    <t>{from:1; to:2; chat_text: text, chat_on: date_time}</t>
   </si>
   <si>
     <t xml:space="preserve">Highlighted Users </t>
@@ -285,12 +276,87 @@
   <si>
     <t>Plan read</t>
   </si>
+  <si>
+    <t>user_id : 1; talent_category:'talent_id'</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "data": [
+        {
+            "user_id": "user_id",
+            "user_name": "username",
+            "photos": "image_name1, image_name2",
+            "videos": "video_url1, video_url2",
+            "photo_dir_url": "image_dir_url"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+ "from_user_id":"3", 
+ "to_user_id":"4",
+ "chat_text": "test chat"
+}</t>
+  </si>
+  <si>
+    <t>{"status":"success","message":"Chat submitted successfully"}</t>
+  </si>
+  <si>
+    <t>http://celebritybe.local/api/v1/userchat</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "data": [
+        {
+            "chat_id": "11",
+            "chat_from": "3",
+            "chat_to": "5",
+            "chat_text": "test chat",
+            "chat_lock": "0",
+            "chat_on": "2018-02-15 18:14:56",
+            "chat_read_on": "0000-00-00 00:00:00",
+            "id": "4",
+            "user_id": "3",
+            "first_name": "Vivek",
+            "middle_name": "",
+            "last_name": "PP",
+            "display_name": "vivek",
+            "dob": "1990-12-03",
+            "gender": "male",
+            "nationality": "1",
+            "state": "1",
+            "city": "1",
+            "location": "kaloor",
+            "address": "Sample addres,Kaloor,Kochi",
+            "phone": "9048809095",
+            "mobile": "9048809095",
+            "email": "vivek@gmail.com",
+            "associations": "",
+            "talent_category": "10",
+            "description": "Ask Different is a question and answer site for power users of Apple hardware and software. Join them; it only takes a minute",
+            "tags_interest": "film making, short films, photography",
+            "photos": "3_5.jpg,3_6.jpg",
+            "videos": "https://www.youtube.com/watch?v=iz0wKv9mDJI,https://www.youtube.com/watch?v=iz0wKv9mDJI",
+            "photos_moderate": "0",
+            "videos_moderate": "0",
+            "links": "",
+            "experience": "5",
+            "subscription_id": "0",
+            "modified_on": "2018-01-27 10:42:50",
+            "modified_by": "2018-01-27 10:42:50"
+        }
+    ]
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -317,6 +383,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -360,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,6 +494,15 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -787,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -798,9 +879,9 @@
     <col min="3" max="3" width="50.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="2"/>
     <col min="5" max="5" width="50.42578125" style="3"/>
-    <col min="6" max="6" width="31.28515625" style="3"/>
+    <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="31.5703125"/>
-    <col min="8" max="8" width="17.7109375"/>
+    <col min="8" max="8" width="49.42578125" customWidth="1"/>
     <col min="9" max="9" width="42.28515625"/>
     <col min="10" max="1025" width="8.5703125"/>
   </cols>
@@ -898,7 +979,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7"/>
@@ -919,7 +1000,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -929,10 +1010,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>19</v>
@@ -942,7 +1023,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -952,46 +1033,46 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="20">
+    <row r="8" spans="1:9" s="7" customFormat="1">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="B8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" s="9" customFormat="1">
       <c r="A9" s="11">
@@ -1034,7 +1115,7 @@
         <v>20</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1057,17 +1138,17 @@
         <v>20</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" s="9" customFormat="1">
+    <row r="12" spans="1:9" s="9" customFormat="1" ht="75">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>27</v>
@@ -1076,11 +1157,11 @@
         <v>19</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="23" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -1101,7 +1182,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1122,7 +1203,7 @@
         <v>36</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1142,10 +1223,10 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -1163,12 +1244,11 @@
       <c r="D16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1187,7 +1267,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1208,52 +1288,60 @@
         <v>36</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="20">
+    <row r="19" spans="1:9" s="9" customFormat="1">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="20">
+      <c r="C19" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="E19" s="7"/>
+      <c r="F19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" s="9" customFormat="1">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="C20" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="20">
@@ -1263,7 +1351,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="5"/>
@@ -1271,7 +1359,7 @@
         <v>36</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1281,10 +1369,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="5"/>
@@ -1292,7 +1380,7 @@
         <v>43</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>

</xml_diff>

<commit_message>
Interview API commit: * Interview GET & POST APIs * Updated in APIs.xlsx
</commit_message>
<xml_diff>
--- a/db/APIs.xlsx
+++ b/db/APIs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>#</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Chat_messages</t>
   </si>
   <si>
-    <t>{user_id : 1;}</t>
-  </si>
-  <si>
     <t>chat submit</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
   </si>
   <si>
     <t>Send Interview letters</t>
-  </si>
-  <si>
-    <t>http://celebritybe.local/api/v1/interview-submit</t>
   </si>
   <si>
     <t>http://celebritybe.local/api/v1/interviews</t>
@@ -350,6 +344,25 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>{
+ "to" : "9",
+ "from" : "3",
+ "interview_data" : {
+  "intrw_subject"  : "interview subject",
+  "intrw_on"    : "2018-02-17 20:30",
+  "intrw_due"   : "2018-02-18 20:30",
+  "intrw_location"  : "interview location",
+  "intrw_description" : "interview description",
+  "oganizer_name"  : "Test company",  
+  "oganizer_contact"  : "Test contact",
+  "oganizer_website"  : "www.organization.com"
+ }
+}</t>
+  </si>
+  <si>
+    <t>{"status":true,"msg":"Interview has been successfully scheduled!","action":"interview"}</t>
   </si>
 </sst>
 </file>
@@ -432,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,9 +507,6 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -868,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,7 +989,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7"/>
@@ -1000,7 +1010,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1010,10 +1020,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>19</v>
@@ -1023,7 +1033,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -1033,20 +1043,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1056,10 +1066,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>19</v>
@@ -1068,10 +1078,10 @@
         <v>20</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="9" customFormat="1">
@@ -1115,7 +1125,7 @@
         <v>20</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1138,17 +1148,17 @@
         <v>20</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" s="9" customFormat="1" ht="75">
+    <row r="12" spans="1:9" s="9" customFormat="1">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>27</v>
@@ -1157,11 +1167,11 @@
         <v>19</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -1182,7 +1192,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1203,7 +1213,7 @@
         <v>36</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1223,10 +1233,10 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -1248,7 +1258,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1267,7 +1277,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1280,7 +1290,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="5"/>
@@ -1288,7 +1298,7 @@
         <v>36</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1301,20 +1311,20 @@
         <v>42</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="24" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I19" s="7"/>
     </row>
@@ -1323,67 +1333,73 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="24"/>
+        <v>57</v>
+      </c>
+      <c r="F20" s="23"/>
       <c r="G20" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="20">
+    <row r="21" spans="1:9" s="9" customFormat="1">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5" t="s">
+      <c r="C21" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="20">
+      <c r="G21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" s="9" customFormat="1">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="D22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="7"/>
     </row>
     <row r="24" spans="1:9">
       <c r="C24" s="6"/>
@@ -1405,7 +1421,7 @@
     <hyperlink ref="C19" r:id="rId13"/>
     <hyperlink ref="C20" r:id="rId14"/>
     <hyperlink ref="C21" r:id="rId15"/>
-    <hyperlink ref="C22" r:id="rId16" display="http://celebritybe.local/api/v1/interviews"/>
+    <hyperlink ref="C22" r:id="rId16"/>
     <hyperlink ref="C6" r:id="rId17"/>
     <hyperlink ref="C13" r:id="rId18"/>
     <hyperlink ref="C7" r:id="rId19" display="http://celebritybe.local/api/v1/userimages"/>

</xml_diff>

<commit_message>
chatusers get method commit: * created chatusers get method
</commit_message>
<xml_diff>
--- a/db/APIs.xlsx
+++ b/db/APIs.xlsx
@@ -296,9 +296,6 @@
   </si>
   <si>
     <t>{"status":"success","message":"Chat submitted successfully"}</t>
-  </si>
-  <si>
-    <t>http://celebritybe.local/api/v1/userchat</t>
   </si>
   <si>
     <t>{
@@ -363,6 +360,9 @@
   </si>
   <si>
     <t>{"status":true,"msg":"Interview has been successfully scheduled!","action":"interview"}</t>
+  </si>
+  <si>
+    <t>http://celebritybe.local/api/v1/userchats</t>
   </si>
 </sst>
 </file>
@@ -879,7 +879,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1311,7 +1311,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>19</v>
@@ -1324,7 +1324,7 @@
         <v>53</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I19" s="7"/>
     </row>
@@ -1336,7 +1336,7 @@
         <v>43</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>11</v>
@@ -1390,14 +1390,14 @@
         <v>11</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I22" s="7"/>
     </row>

</xml_diff>

<commit_message>
Count APIs commit: * interest count * interview count * visit count * chatuser count
</commit_message>
<xml_diff>
--- a/db/APIs.xlsx
+++ b/db/APIs.xlsx
@@ -285,13 +285,6 @@
             "photo_dir_url": "image_dir_url"
         }
     ]
-}</t>
-  </si>
-  <si>
-    <t>{
- "from_user_id":"3", 
- "to_user_id":"4",
- "chat_text": "test chat"
 }</t>
   </si>
   <si>
@@ -363,6 +356,13 @@
   </si>
   <si>
     <t>http://celebritybe.local/api/v1/userchats</t>
+  </si>
+  <si>
+    <t>{
+ "chat_from":"4", 
+ "chat_to":"3",
+ "chat_text": "new chat"
+}</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+      <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1197,26 +1197,26 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="20">
+    <row r="14" spans="1:9" s="9" customFormat="1">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1">
       <c r="A15" s="11">
@@ -1303,7 +1303,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" s="9" customFormat="1">
+    <row r="19" spans="1:9" s="9" customFormat="1" ht="60.75">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>19</v>
@@ -1324,7 +1324,7 @@
         <v>53</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I19" s="7"/>
     </row>
@@ -1336,20 +1336,20 @@
         <v>43</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="7" t="s">
         <v>53</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I20" s="7"/>
     </row>
@@ -1390,14 +1390,14 @@
         <v>11</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I22" s="7"/>
     </row>

</xml_diff>

<commit_message>
APIs.xlsx file updates: * Included dp image update option
</commit_message>
<xml_diff>
--- a/db/APIs.xlsx
+++ b/db/APIs.xlsx
@@ -252,9 +252,6 @@
     <t>http://celebritybe.local/api/v1/usermedias</t>
   </si>
   <si>
-    <t>Show featured media</t>
-  </si>
-  <si>
     <t>Add featured media</t>
   </si>
   <si>
@@ -272,20 +269,6 @@
   </si>
   <si>
     <t>user_id : 1; talent_category:'talent_id'</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
-    "data": [
-        {
-            "user_id": "user_id",
-            "user_name": "username",
-            "photos": "image_name1, image_name2",
-            "videos": "video_url1, video_url2",
-            "photo_dir_url": "image_dir_url"
-        }
-    ]
-}</t>
   </si>
   <si>
     <t>{"status":"success","message":"Chat submitted successfully"}</t>
@@ -363,6 +346,18 @@
  "chat_to":"3",
  "chat_text": "new chat"
 }</t>
+  </si>
+  <si>
+    <t>{
+ "user_id" : "user_id",
+ "dp_image" : "dp_image_name",
+ "old_video_indx" : "old_video_url_index",
+ "new_user_video" : "new_video_url",
+ "old_image_name" : "old_image_name",
+ "new_user_image" : "base64 image data"</t>
+  </si>
+  <si>
+    <t>{"status":true,"message":"User media update successfull"}</t>
   </si>
 </sst>
 </file>
@@ -445,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -511,6 +506,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -878,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -989,7 +987,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7"/>
@@ -1010,7 +1008,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1033,17 +1031,17 @@
         <v>20</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" s="9" customFormat="1">
+    <row r="7" spans="1:9" s="9" customFormat="1" ht="75">
       <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>49</v>
@@ -1051,19 +1049,19 @@
       <c r="D7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>52</v>
+      <c r="E7" s="25" t="s">
+        <v>51</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="7" customFormat="1">
+    <row r="8" spans="1:9" s="9" customFormat="1" ht="105">
       <c r="A8" s="11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>50</v>
@@ -1072,17 +1070,19 @@
         <v>49</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>56</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" s="9" customFormat="1">
       <c r="A9" s="11">
@@ -1125,7 +1125,7 @@
         <v>20</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1148,7 +1148,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1158,7 +1158,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>27</v>
@@ -1171,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -1192,7 +1192,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1213,7 +1213,7 @@
         <v>36</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -1233,10 +1233,10 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -1258,7 +1258,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1277,7 +1277,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1298,7 +1298,7 @@
         <v>36</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -1311,7 +1311,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>19</v>
@@ -1321,10 +1321,10 @@
         <v>20</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I19" s="7"/>
     </row>
@@ -1336,20 +1336,20 @@
         <v>43</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I20" s="7"/>
     </row>
@@ -1371,7 +1371,7 @@
         <v>36</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -1390,14 +1390,14 @@
         <v>11</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I22" s="7"/>
     </row>
@@ -1425,8 +1425,8 @@
     <hyperlink ref="C6" r:id="rId17"/>
     <hyperlink ref="C13" r:id="rId18"/>
     <hyperlink ref="C7" r:id="rId19" display="http://celebritybe.local/api/v1/userimages"/>
-    <hyperlink ref="C8" r:id="rId20" display="http://celebritybe.local/api/v1/userimages"/>
-    <hyperlink ref="C12" r:id="rId21"/>
+    <hyperlink ref="C12" r:id="rId20"/>
+    <hyperlink ref="C8" r:id="rId21" display="http://celebritybe.local/api/v1/userimages"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>

</xml_diff>